<commit_message>
plus code e endereco unidos
</commit_message>
<xml_diff>
--- a/Lojas/Juntando Tudo/Enderecos_Processados.xlsx
+++ b/Lojas/Juntando Tudo/Enderecos_Processados.xlsx
@@ -457,7 +457,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -509,7 +509,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>4049</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -613,7 +613,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>1.400</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -665,7 +665,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -816,7 +816,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>334</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -868,7 +868,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Av. Luís Viana Filho, 3056</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -920,7 +920,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>119</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -972,7 +972,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>516</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>227</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -1071,12 +1071,12 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>9/11 - Calçada</t>
+          <t>- 9/11 - Calçada</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>9/11</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -1123,7 +1123,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>225</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -1274,7 +1274,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -1319,11 +1319,6 @@
           <t>Federação</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>8a</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1363,7 +1358,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -1410,7 +1405,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1452,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -1499,7 +1494,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -1541,7 +1536,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>n65</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -1588,7 +1583,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>289</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -1640,7 +1635,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -1692,7 +1687,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -1734,7 +1729,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>numero 276</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -1875,7 +1870,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>808</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -1910,11 +1905,6 @@
           <t>avn</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>Rua Engenheiro Almiro Queiroz - Federação</t>
-        </is>
-      </c>
       <c r="J32" t="inlineStr">
         <is>
           <t>Salvador</t>
@@ -1969,7 +1959,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2016,7 +2006,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2110,7 +2100,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>427</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2162,7 +2152,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>74</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2204,7 +2194,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Estação da Lapa, 35</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2246,7 +2236,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>113</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2402,7 +2392,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2449,7 +2439,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2484,16 +2474,6 @@
           <t>DAM AVELAR</t>
         </is>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>CEP: 41.315-370 Logradouro: R Dos Beneditinos Número: 12 D Complemento: Terreo Bairro: Dom Avelar Município:</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>R. dos Beneditinos, 12d</t>
-        </is>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2538,7 +2518,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2585,7 +2565,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>1050</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2617,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2684,7 +2664,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2716,12 +2696,12 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>1o Andar - Matatu</t>
+          <t>- 1o Andar - Matatu</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>637</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2768,7 +2748,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2810,7 +2790,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2852,7 +2832,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>309</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2904,7 +2884,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>807</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -2998,7 +2978,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -3040,7 +3020,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>199</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -3087,7 +3067,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>400</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -3129,7 +3109,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>205</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -3176,7 +3156,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -3223,7 +3203,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>597</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -3263,11 +3243,6 @@
           <t>Praça da Piedade</t>
         </is>
       </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>632</t>
-        </is>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3317,7 +3292,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -3364,7 +3339,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -3411,7 +3386,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>95</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -3458,7 +3433,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>139</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -3584,7 +3559,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -3631,7 +3606,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>712 ZY, Térreo, Nº 11</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -3673,7 +3648,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>959</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -3826,7 +3801,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -3868,7 +3843,7 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>N119</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -4073,7 +4048,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -4125,7 +4100,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>2006</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -4172,7 +4147,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>430 Shopping Bonocô Center, Loja 16</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -4219,7 +4194,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -4261,7 +4236,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -4308,7 +4283,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -4385,16 +4360,6 @@
           <t>R. Sérgio de Carvalho, 2andar</t>
         </is>
       </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>2andar - Federação</t>
-        </is>
-      </c>
-      <c r="J87" t="inlineStr">
-        <is>
-          <t>2andar</t>
-        </is>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4444,7 +4409,7 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>457</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -4513,12 +4478,12 @@
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>Loja B 520 - Daniel Lisboa</t>
+          <t>- Loja B 520 - Daniel Lisboa</t>
         </is>
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>780</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -4565,7 +4530,7 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>753</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -4654,7 +4619,7 @@
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>385</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -4696,12 +4661,12 @@
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>Térreo - Nazaré</t>
+          <t>- Térreo - Nazaré</t>
         </is>
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>no 117</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -4746,11 +4711,6 @@
           <t>BA</t>
         </is>
       </c>
-      <c r="J95" t="inlineStr">
-        <is>
-          <t>R. da Mouraria, 31, Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4817,7 +4777,7 @@
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>R. Joaquim Calado, 0005</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -4869,7 +4829,7 @@
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -4933,12 +4893,12 @@
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>Sala 904 - Caminho das Árvores</t>
+          <t>- Sala 904 - Caminho das Árvores</t>
         </is>
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>939</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -4985,7 +4945,7 @@
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -5027,7 +4987,7 @@
       </c>
       <c r="J102" t="inlineStr">
         <is>
-          <t>342</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -5101,7 +5061,7 @@
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>180</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -5148,7 +5108,7 @@
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>68 B</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -5195,12 +5155,12 @@
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>Loja 100</t>
+          <t>- Barris</t>
         </is>
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>2º Piso, Rua Conselheiro Junqueira Ayres, 165</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -5247,7 +5207,7 @@
       </c>
       <c r="J107" t="inlineStr">
         <is>
-          <t>412</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -5294,12 +5254,12 @@
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>F - Engenho Velho de Brotas</t>
+          <t>- F - Engenho Velho de Brotas</t>
         </is>
       </c>
       <c r="J108" t="inlineStr">
         <is>
-          <t>1179</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -5363,12 +5323,12 @@
       </c>
       <c r="I110" t="inlineStr">
         <is>
-          <t>KM 7 - Pirajá</t>
+          <t>- KM 7 - Pirajá</t>
         </is>
       </c>
       <c r="J110" t="inlineStr">
         <is>
-          <t>9069</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -5415,12 +5375,12 @@
       </c>
       <c r="I111" t="inlineStr">
         <is>
-          <t>Andar: G2</t>
+          <t>Loja 5015 - Caminho das Árvores</t>
         </is>
       </c>
       <c r="J111" t="inlineStr">
         <is>
-          <t>Salvador Shopping, 3133</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -5455,11 +5415,6 @@
           <t>avn</t>
         </is>
       </c>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>Rua Engenheiro Almiro Queiroz - Federação</t>
-        </is>
-      </c>
       <c r="J112" t="inlineStr">
         <is>
           <t>Salvador</t>
@@ -5509,7 +5464,7 @@
       </c>
       <c r="J113" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -5682,7 +5637,7 @@
       </c>
       <c r="J117" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -5729,12 +5684,12 @@
       </c>
       <c r="I118" t="inlineStr">
         <is>
-          <t>1º Andar - Caminho das Árvores</t>
+          <t>- 1º Andar - Caminho das Árvores</t>
         </is>
       </c>
       <c r="J118" t="inlineStr">
         <is>
-          <t>3133</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -5781,7 +5736,7 @@
       </c>
       <c r="J119" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -5865,7 +5820,7 @@
       </c>
       <c r="J121" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -5912,7 +5867,7 @@
       </c>
       <c r="J122" t="inlineStr">
         <is>
-          <t>532</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -5959,7 +5914,7 @@
       </c>
       <c r="J123" t="inlineStr">
         <is>
-          <t>1470</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -6095,7 +6050,7 @@
       </c>
       <c r="J126" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -6189,7 +6144,7 @@
       </c>
       <c r="J128" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -6236,7 +6191,7 @@
       </c>
       <c r="J129" t="inlineStr">
         <is>
-          <t>71</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -6288,7 +6243,7 @@
       </c>
       <c r="J130" t="inlineStr">
         <is>
-          <t>3570</t>
+          <t>Lauro de Freitas</t>
         </is>
       </c>
     </row>
@@ -6340,7 +6295,7 @@
       </c>
       <c r="J131" t="inlineStr">
         <is>
-          <t>853</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -6392,7 +6347,7 @@
       </c>
       <c r="J132" t="inlineStr">
         <is>
-          <t>964</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -6444,7 +6399,7 @@
       </c>
       <c r="J133" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -6538,7 +6493,7 @@
       </c>
       <c r="J135" t="inlineStr">
         <is>
-          <t>92 LOJA 45, PISO 2</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -6585,7 +6540,7 @@
       </c>
       <c r="J136" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -6637,7 +6592,7 @@
       </c>
       <c r="J137" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -6679,12 +6634,12 @@
       </c>
       <c r="I138" t="inlineStr">
         <is>
-          <t>Loja 277 - Barra</t>
+          <t>- Loja 277 - Barra</t>
         </is>
       </c>
       <c r="J138" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -6726,12 +6681,12 @@
       </c>
       <c r="I139" t="inlineStr">
         <is>
-          <t>Loja 62 - Barra</t>
+          <t>- Loja 62 - Barra</t>
         </is>
       </c>
       <c r="J139" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -6778,7 +6733,7 @@
       </c>
       <c r="J140" t="inlineStr">
         <is>
-          <t>155</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -6825,12 +6780,12 @@
       </c>
       <c r="I141" t="inlineStr">
         <is>
-          <t>Loja 155 - Barra</t>
+          <t>- Loja 155 - Barra</t>
         </is>
       </c>
       <c r="J141" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -6872,12 +6827,12 @@
       </c>
       <c r="I142" t="inlineStr">
         <is>
-          <t>Loja 5 - Barra</t>
+          <t>- Loja 5 - Barra</t>
         </is>
       </c>
       <c r="J142" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -6924,7 +6879,7 @@
       </c>
       <c r="J143" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -6976,7 +6931,7 @@
       </c>
       <c r="J144" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7028,7 +6983,7 @@
       </c>
       <c r="J145" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7070,12 +7025,12 @@
       </c>
       <c r="I146" t="inlineStr">
         <is>
-          <t>Loja 87 - Barra</t>
+          <t>- Loja 87 - Barra</t>
         </is>
       </c>
       <c r="J146" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7122,12 +7077,12 @@
       </c>
       <c r="I147" t="inlineStr">
         <is>
-          <t>Loja 278 - Barra</t>
+          <t>- Loja 278 - Barra</t>
         </is>
       </c>
       <c r="J147" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7169,12 +7124,12 @@
       </c>
       <c r="I148" t="inlineStr">
         <is>
-          <t>Chame-Chame</t>
+          <t>- Chame-Chame</t>
         </is>
       </c>
       <c r="J148" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7221,7 +7176,7 @@
       </c>
       <c r="J149" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7268,7 +7223,7 @@
       </c>
       <c r="J150" t="inlineStr">
         <is>
-          <t>3133</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7315,12 +7270,12 @@
       </c>
       <c r="I151" t="inlineStr">
         <is>
-          <t>Loja 273 - Barra</t>
+          <t>- Loja 273 - Barra</t>
         </is>
       </c>
       <c r="J151" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7362,12 +7317,12 @@
       </c>
       <c r="I152" t="inlineStr">
         <is>
-          <t>Loja 141 - Barra</t>
+          <t>- Loja 141 - Barra</t>
         </is>
       </c>
       <c r="J152" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7414,12 +7369,12 @@
       </c>
       <c r="I153" t="inlineStr">
         <is>
-          <t>Loja 2 - Barra</t>
+          <t>- Loja 2 - Barra</t>
         </is>
       </c>
       <c r="J153" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7471,7 +7426,7 @@
       </c>
       <c r="J154" t="inlineStr">
         <is>
-          <t>3133 Salvador Shopping Piso L1</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7523,7 +7478,7 @@
       </c>
       <c r="J155" t="inlineStr">
         <is>
-          <t>3133</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7565,12 +7520,12 @@
       </c>
       <c r="I156" t="inlineStr">
         <is>
-          <t>Loja 75 - Barra</t>
+          <t>- Loja 75 - Barra</t>
         </is>
       </c>
       <c r="J156" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7617,12 +7572,12 @@
       </c>
       <c r="I157" t="inlineStr">
         <is>
-          <t>Chame-Chame</t>
+          <t>- Chame-Chame</t>
         </is>
       </c>
       <c r="J157" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7664,12 +7619,12 @@
       </c>
       <c r="I158" t="inlineStr">
         <is>
-          <t>Loja 272 - Barra</t>
+          <t>- Loja 272 - Barra</t>
         </is>
       </c>
       <c r="J158" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7716,12 +7671,12 @@
       </c>
       <c r="I159" t="inlineStr">
         <is>
-          <t>Loja 235 - Barra</t>
+          <t>- Loja 235 - Barra</t>
         </is>
       </c>
       <c r="J159" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7763,12 +7718,12 @@
       </c>
       <c r="I160" t="inlineStr">
         <is>
-          <t>Loja 15 - Barra</t>
+          <t>- Loja 15 - Barra</t>
         </is>
       </c>
       <c r="J160" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7810,12 +7765,12 @@
       </c>
       <c r="I161" t="inlineStr">
         <is>
-          <t>Loja 152 - Barra</t>
+          <t>- Loja 152 - Barra</t>
         </is>
       </c>
       <c r="J161" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7862,12 +7817,12 @@
       </c>
       <c r="I162" t="inlineStr">
         <is>
-          <t>Loja 82 - Barra</t>
+          <t>- Loja 82 - Barra</t>
         </is>
       </c>
       <c r="J162" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7909,12 +7864,12 @@
       </c>
       <c r="I163" t="inlineStr">
         <is>
-          <t>Loja 56 - Barra</t>
+          <t>- Loja 56 - Barra</t>
         </is>
       </c>
       <c r="J163" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -7966,7 +7921,7 @@
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8013,7 +7968,7 @@
       </c>
       <c r="J165" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8060,7 +8015,7 @@
       </c>
       <c r="J166" t="inlineStr">
         <is>
-          <t>836</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8102,12 +8057,12 @@
       </c>
       <c r="I167" t="inlineStr">
         <is>
-          <t>Loja 124 - Barra</t>
+          <t>- Loja 124 - Barra</t>
         </is>
       </c>
       <c r="J167" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8154,12 +8109,12 @@
       </c>
       <c r="I168" t="inlineStr">
         <is>
-          <t>Loja 154 - Barra</t>
+          <t>- Loja 154 - Barra</t>
         </is>
       </c>
       <c r="J168" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8201,12 +8156,12 @@
       </c>
       <c r="I169" t="inlineStr">
         <is>
-          <t>Loja 135 - Barra</t>
+          <t>- Loja 135 - Barra</t>
         </is>
       </c>
       <c r="J169" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8253,12 +8208,12 @@
       </c>
       <c r="I170" t="inlineStr">
         <is>
-          <t>Loja 217 - Barra</t>
+          <t>- Loja 217 - Barra</t>
         </is>
       </c>
       <c r="J170" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8310,7 +8265,7 @@
       </c>
       <c r="J171" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8357,12 +8312,12 @@
       </c>
       <c r="I172" t="inlineStr">
         <is>
-          <t>Loja 7 - Barra</t>
+          <t>- Loja 7 - Barra</t>
         </is>
       </c>
       <c r="J172" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8409,12 +8364,12 @@
       </c>
       <c r="I173" t="inlineStr">
         <is>
-          <t>Loja 261 - Barra</t>
+          <t>- Loja 261 - Barra</t>
         </is>
       </c>
       <c r="J173" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8456,12 +8411,12 @@
       </c>
       <c r="I174" t="inlineStr">
         <is>
-          <t>Loja 119 - Barra</t>
+          <t>- Loja 119 - Barra</t>
         </is>
       </c>
       <c r="J174" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8508,12 +8463,12 @@
       </c>
       <c r="I175" t="inlineStr">
         <is>
-          <t>loja 352/353 - Barra</t>
+          <t>- loja 352/353 - Barra</t>
         </is>
       </c>
       <c r="J175" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8565,7 +8520,7 @@
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8612,12 +8567,12 @@
       </c>
       <c r="I177" t="inlineStr">
         <is>
-          <t>Loja 71 - Barra</t>
+          <t>- Loja 71 - Barra</t>
         </is>
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8659,12 +8614,12 @@
       </c>
       <c r="I178" t="inlineStr">
         <is>
-          <t>Loja 10 - Barra</t>
+          <t>- Loja 10 - Barra</t>
         </is>
       </c>
       <c r="J178" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8716,7 +8671,7 @@
       </c>
       <c r="J179" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8758,12 +8713,12 @@
       </c>
       <c r="I180" t="inlineStr">
         <is>
-          <t>Loja 63 - Barra</t>
+          <t>- Loja 63 - Barra</t>
         </is>
       </c>
       <c r="J180" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8805,12 +8760,12 @@
       </c>
       <c r="I181" t="inlineStr">
         <is>
-          <t>Loja 437 - Barra</t>
+          <t>- Loja 437 - Barra</t>
         </is>
       </c>
       <c r="J181" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8852,12 +8807,12 @@
       </c>
       <c r="I182" t="inlineStr">
         <is>
-          <t>Loja 274 - Barra</t>
+          <t>- Loja 274 - Barra</t>
         </is>
       </c>
       <c r="J182" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8894,7 +8849,7 @@
       </c>
       <c r="J183" t="inlineStr">
         <is>
-          <t>316</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8941,12 +8896,12 @@
       </c>
       <c r="I184" t="inlineStr">
         <is>
-          <t>Loja 275 - Barra</t>
+          <t>- Loja 275 - Barra</t>
         </is>
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -8998,7 +8953,7 @@
       </c>
       <c r="J185" t="inlineStr">
         <is>
-          <t>3133</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9040,12 +8995,12 @@
       </c>
       <c r="I186" t="inlineStr">
         <is>
-          <t>Loja 184 - Barra</t>
+          <t>- Loja 184 - Barra</t>
         </is>
       </c>
       <c r="J186" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9092,7 +9047,7 @@
       </c>
       <c r="J187" t="inlineStr">
         <is>
-          <t>09</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9144,7 +9099,7 @@
       </c>
       <c r="J188" t="inlineStr">
         <is>
-          <t>282</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9196,7 +9151,7 @@
       </c>
       <c r="J189" t="inlineStr">
         <is>
-          <t>774</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9248,7 +9203,7 @@
       </c>
       <c r="J190" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9290,12 +9245,12 @@
       </c>
       <c r="I191" t="inlineStr">
         <is>
-          <t>208 - Caminho das Árvores</t>
+          <t>- 208 - Caminho das Árvores</t>
         </is>
       </c>
       <c r="J191" t="inlineStr">
         <is>
-          <t>3133</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9337,12 +9292,12 @@
       </c>
       <c r="I192" t="inlineStr">
         <is>
-          <t>Loja 280 - Barra</t>
+          <t>- Loja 280 - Barra</t>
         </is>
       </c>
       <c r="J192" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9384,12 +9339,12 @@
       </c>
       <c r="I193" t="inlineStr">
         <is>
-          <t>Loja 245 - Barra</t>
+          <t>- Loja 245 - Barra</t>
         </is>
       </c>
       <c r="J193" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9441,7 +9396,7 @@
       </c>
       <c r="J194" t="inlineStr">
         <is>
-          <t>300</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9483,12 +9438,12 @@
       </c>
       <c r="I195" t="inlineStr">
         <is>
-          <t>Loja 53 - Barra</t>
+          <t>- Loja 53 - Barra</t>
         </is>
       </c>
       <c r="J195" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9540,7 +9495,7 @@
       </c>
       <c r="J196" t="inlineStr">
         <is>
-          <t>Av. Centenário, 2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9582,12 +9537,12 @@
       </c>
       <c r="I197" t="inlineStr">
         <is>
-          <t>Loja 38 - Barra</t>
+          <t>- Loja 38 - Barra</t>
         </is>
       </c>
       <c r="J197" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9634,7 +9589,7 @@
       </c>
       <c r="J198" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9676,12 +9631,12 @@
       </c>
       <c r="I199" t="inlineStr">
         <is>
-          <t>OT - Iapi</t>
+          <t>- OT - Iapi</t>
         </is>
       </c>
       <c r="J199" t="inlineStr">
         <is>
-          <t>93</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9728,7 +9683,7 @@
       </c>
       <c r="J200" t="inlineStr">
         <is>
-          <t>357</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9770,12 +9725,12 @@
       </c>
       <c r="I201" t="inlineStr">
         <is>
-          <t>Loja 164 - Barra</t>
+          <t>- Loja 164 - Barra</t>
         </is>
       </c>
       <c r="J201" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9822,7 +9777,7 @@
       </c>
       <c r="J202" t="inlineStr">
         <is>
-          <t>298</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9911,12 +9866,12 @@
       </c>
       <c r="I204" t="inlineStr">
         <is>
-          <t>Loja 209 - Barra</t>
+          <t>- Loja 209 - Barra</t>
         </is>
       </c>
       <c r="J204" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -9963,12 +9918,12 @@
       </c>
       <c r="I205" t="inlineStr">
         <is>
-          <t>Loja 293 - Barra</t>
+          <t>- Loja 293 - Barra</t>
         </is>
       </c>
       <c r="J205" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10020,7 +9975,7 @@
       </c>
       <c r="J206" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10057,12 +10012,12 @@
       </c>
       <c r="I207" t="inlineStr">
         <is>
-          <t>Loja 192 - Barra</t>
+          <t>- Loja 192 - Barra</t>
         </is>
       </c>
       <c r="J207" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10151,7 +10106,7 @@
       </c>
       <c r="J209" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10198,12 +10153,12 @@
       </c>
       <c r="I210" t="inlineStr">
         <is>
-          <t>Loja 190 - Barra</t>
+          <t>- Loja 190 - Barra</t>
         </is>
       </c>
       <c r="J210" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10255,7 +10210,7 @@
       </c>
       <c r="J211" t="inlineStr">
         <is>
-          <t>370</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10302,12 +10257,12 @@
       </c>
       <c r="I212" t="inlineStr">
         <is>
-          <t>E 94 - Calçada</t>
+          <t>- E 94 - Calçada</t>
         </is>
       </c>
       <c r="J212" t="inlineStr">
         <is>
-          <t>92</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10354,12 +10309,12 @@
       </c>
       <c r="I213" t="inlineStr">
         <is>
-          <t>Loja 92 - Barra</t>
+          <t>- Loja 92 - Barra</t>
         </is>
       </c>
       <c r="J213" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10411,7 +10366,7 @@
       </c>
       <c r="J214" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10448,12 +10403,12 @@
       </c>
       <c r="I215" t="inlineStr">
         <is>
-          <t>Loja 215 - Barra</t>
+          <t>- Loja 215 - Barra</t>
         </is>
       </c>
       <c r="J215" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10495,12 +10450,12 @@
       </c>
       <c r="I216" t="inlineStr">
         <is>
-          <t>Loja 49 - Barra</t>
+          <t>- Loja 49 - Barra</t>
         </is>
       </c>
       <c r="J216" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10542,12 +10497,12 @@
       </c>
       <c r="I217" t="inlineStr">
         <is>
-          <t>Loja 26 - Barra</t>
+          <t>- Loja 26 - Barra</t>
         </is>
       </c>
       <c r="J217" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10589,12 +10544,12 @@
       </c>
       <c r="I218" t="inlineStr">
         <is>
-          <t>Loja 76 - Barra</t>
+          <t>- Loja 76 - Barra</t>
         </is>
       </c>
       <c r="J218" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10641,12 +10596,12 @@
       </c>
       <c r="I219" t="inlineStr">
         <is>
-          <t>Loja 171 - Barra</t>
+          <t>- Loja 171 - Barra</t>
         </is>
       </c>
       <c r="J219" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10698,7 +10653,7 @@
       </c>
       <c r="J220" t="inlineStr">
         <is>
-          <t>284</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10745,7 +10700,7 @@
       </c>
       <c r="J221" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10780,11 +10735,6 @@
           <t>Estrada Campinas Piraja,0,Campinas</t>
         </is>
       </c>
-      <c r="I222" t="inlineStr">
-        <is>
-          <t>41270000</t>
-        </is>
-      </c>
       <c r="J222" t="inlineStr">
         <is>
           <t>Salvador</t>
@@ -10829,12 +10779,12 @@
       </c>
       <c r="I223" t="inlineStr">
         <is>
-          <t>Loja 260 - Barra</t>
+          <t>- Loja 260 - Barra</t>
         </is>
       </c>
       <c r="J223" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10886,7 +10836,7 @@
       </c>
       <c r="J224" t="inlineStr">
         <is>
-          <t>305</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10928,12 +10878,12 @@
       </c>
       <c r="I225" t="inlineStr">
         <is>
-          <t>Loja 105 - Barra</t>
+          <t>- Loja 105 - Barra</t>
         </is>
       </c>
       <c r="J225" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -10980,12 +10930,12 @@
       </c>
       <c r="I226" t="inlineStr">
         <is>
-          <t>Cajazeiras 8</t>
+          <t>- Cajazeiras 8</t>
         </is>
       </c>
       <c r="J226" t="inlineStr">
         <is>
-          <t>1400</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11027,12 +10977,12 @@
       </c>
       <c r="I227" t="inlineStr">
         <is>
-          <t>Loja 221 - Barra</t>
+          <t>- Loja 221 - Barra</t>
         </is>
       </c>
       <c r="J227" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11074,12 +11024,12 @@
       </c>
       <c r="I228" t="inlineStr">
         <is>
-          <t>Loja 228 - Barra</t>
+          <t>- Loja 228 - Barra</t>
         </is>
       </c>
       <c r="J228" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11121,12 +11071,12 @@
       </c>
       <c r="I229" t="inlineStr">
         <is>
-          <t>Loja 287 - Barra</t>
+          <t>- Loja 287 - Barra</t>
         </is>
       </c>
       <c r="J229" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11178,7 +11128,7 @@
       </c>
       <c r="J230" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11225,12 +11175,12 @@
       </c>
       <c r="I231" t="inlineStr">
         <is>
-          <t>Loja 181 - Barra</t>
+          <t>- Loja 181 - Barra</t>
         </is>
       </c>
       <c r="J231" t="inlineStr">
         <is>
-          <t>2992</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11282,7 +11232,7 @@
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11324,12 +11274,12 @@
       </c>
       <c r="I233" t="inlineStr">
         <is>
-          <t>58 - Barris</t>
+          <t>- 58 - Barris</t>
         </is>
       </c>
       <c r="J233" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11379,11 +11329,6 @@
           <t>Barra</t>
         </is>
       </c>
-      <c r="J234" t="inlineStr">
-        <is>
-          <t>Loja 31, Térreo</t>
-        </is>
-      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -11428,7 +11373,7 @@
       </c>
       <c r="J235" t="inlineStr">
         <is>
-          <t>255</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11480,7 +11425,7 @@
       </c>
       <c r="J236" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11522,7 +11467,7 @@
       </c>
       <c r="J237" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11564,7 +11509,7 @@
       </c>
       <c r="J238" t="inlineStr">
         <is>
-          <t>158</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11611,7 +11556,7 @@
       </c>
       <c r="J239" t="inlineStr">
         <is>
-          <t>321</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11653,12 +11598,12 @@
       </c>
       <c r="I240" t="inlineStr">
         <is>
-          <t>223 - Barris</t>
+          <t>- 223 - Barris</t>
         </is>
       </c>
       <c r="J240" t="inlineStr">
         <is>
-          <t>155</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11757,7 +11702,7 @@
       </c>
       <c r="J242" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11809,7 +11754,7 @@
       </c>
       <c r="J243" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11856,7 +11801,7 @@
       </c>
       <c r="J244" t="inlineStr">
         <is>
-          <t>187</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11898,12 +11843,12 @@
       </c>
       <c r="I245" t="inlineStr">
         <is>
-          <t>Shopping Brotascenter - Brotas</t>
+          <t>- Shopping Brotascenter - Brotas</t>
         </is>
       </c>
       <c r="J245" t="inlineStr">
         <is>
-          <t>1050</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11955,7 +11900,7 @@
       </c>
       <c r="J246" t="inlineStr">
         <is>
-          <t>328</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -11997,12 +11942,12 @@
       </c>
       <c r="I247" t="inlineStr">
         <is>
-          <t>106 - Caminho das Árvores</t>
+          <t>- 106 - Caminho das Árvores</t>
         </is>
       </c>
       <c r="J247" t="inlineStr">
         <is>
-          <t>3133</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12049,7 +11994,7 @@
       </c>
       <c r="J248" t="inlineStr">
         <is>
-          <t>6929</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12101,7 +12046,7 @@
       </c>
       <c r="J249" t="inlineStr">
         <is>
-          <t>354</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12148,7 +12093,7 @@
       </c>
       <c r="J250" t="inlineStr">
         <is>
-          <t>n 400</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12195,7 +12140,7 @@
       </c>
       <c r="J251" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12237,7 +12182,7 @@
       </c>
       <c r="J252" t="inlineStr">
         <is>
-          <t>190</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12289,7 +12234,7 @@
       </c>
       <c r="J253" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12336,7 +12281,7 @@
       </c>
       <c r="J254" t="inlineStr">
         <is>
-          <t>320</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12378,7 +12323,7 @@
       </c>
       <c r="J255" t="inlineStr">
         <is>
-          <t>111</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12477,7 +12422,7 @@
       </c>
       <c r="J257" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12529,7 +12474,7 @@
       </c>
       <c r="J258" t="inlineStr">
         <is>
-          <t>168</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12571,7 +12516,7 @@
       </c>
       <c r="J259" t="inlineStr">
         <is>
-          <t>n 400</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12618,7 +12563,7 @@
       </c>
       <c r="J260" t="inlineStr">
         <is>
-          <t>112</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12702,12 +12647,12 @@
       </c>
       <c r="I262" t="inlineStr">
         <is>
-          <t>Loja 3B - Rio Vermelho</t>
+          <t>- Loja 3B - Rio Vermelho</t>
         </is>
       </c>
       <c r="J262" t="inlineStr">
         <is>
-          <t>87</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12754,7 +12699,7 @@
       </c>
       <c r="J263" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12853,7 +12798,7 @@
       </c>
       <c r="J265" t="inlineStr">
         <is>
-          <t>710</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12895,7 +12840,7 @@
       </c>
       <c r="J266" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12947,7 +12892,7 @@
       </c>
       <c r="J267" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -12989,7 +12934,7 @@
       </c>
       <c r="J268" t="inlineStr">
         <is>
-          <t>211</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -13036,12 +12981,12 @@
       </c>
       <c r="I269" t="inlineStr">
         <is>
-          <t>galeria - Santa Teresa</t>
+          <t>- galeria - Santa Teresa</t>
         </is>
       </c>
       <c r="J269" t="inlineStr">
         <is>
-          <t>177</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -13125,12 +13070,12 @@
       </c>
       <c r="I271" t="inlineStr">
         <is>
-          <t>loja 03 - Graça</t>
+          <t>- loja 03 - Graça</t>
         </is>
       </c>
       <c r="J271" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -13177,7 +13122,7 @@
       </c>
       <c r="J272" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -13224,7 +13169,7 @@
       </c>
       <c r="J273" t="inlineStr">
         <is>
-          <t>587</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -13276,7 +13221,7 @@
       </c>
       <c r="J274" t="inlineStr">
         <is>
-          <t>155</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -13370,7 +13315,7 @@
       </c>
       <c r="J276" t="inlineStr">
         <is>
-          <t>nº7</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -13412,7 +13357,7 @@
       </c>
       <c r="J277" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -13459,7 +13404,7 @@
       </c>
       <c r="J278" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -13511,7 +13456,7 @@
       </c>
       <c r="J279" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -13558,7 +13503,7 @@
       </c>
       <c r="J280" t="inlineStr">
         <is>
-          <t>111</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -13600,12 +13545,12 @@
       </c>
       <c r="I281" t="inlineStr">
         <is>
-          <t>17 - Barris</t>
+          <t>- 17 - Barris</t>
         </is>
       </c>
       <c r="J281" t="inlineStr">
         <is>
-          <t>137</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -13704,7 +13649,7 @@
       </c>
       <c r="J283" t="inlineStr">
         <is>
-          <t>231</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -13756,7 +13701,7 @@
       </c>
       <c r="J284" t="inlineStr">
         <is>
-          <t>131</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -13897,7 +13842,7 @@
       </c>
       <c r="J287" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -13944,7 +13889,7 @@
       </c>
       <c r="J288" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -14043,7 +13988,7 @@
       </c>
       <c r="J290" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -14090,7 +14035,7 @@
       </c>
       <c r="J291" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -14142,7 +14087,7 @@
       </c>
       <c r="J292" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -14189,7 +14134,7 @@
       </c>
       <c r="J293" t="inlineStr">
         <is>
-          <t>165</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -14241,7 +14186,7 @@
       </c>
       <c r="J294" t="inlineStr">
         <is>
-          <t>331</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -14293,7 +14238,7 @@
       </c>
       <c r="J295" t="inlineStr">
         <is>
-          <t>800</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -14345,7 +14290,7 @@
       </c>
       <c r="J296" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -14387,7 +14332,7 @@
       </c>
       <c r="J297" t="inlineStr">
         <is>
-          <t>94</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -14476,7 +14421,7 @@
       </c>
       <c r="J299" t="inlineStr">
         <is>
-          <t>n .34</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -14518,7 +14463,7 @@
       </c>
       <c r="J300" t="inlineStr">
         <is>
-          <t>155</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -14570,7 +14515,7 @@
       </c>
       <c r="J301" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -14622,7 +14567,7 @@
       </c>
       <c r="J302" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -14674,7 +14619,7 @@
       </c>
       <c r="J303" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>
@@ -14768,7 +14713,7 @@
       </c>
       <c r="J305" t="inlineStr">
         <is>
-          <t>979</t>
+          <t>Salvador</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
codigo bom NA ta indo bem
</commit_message>
<xml_diff>
--- a/Lojas/Juntando Tudo/Enderecos_Processados.xlsx
+++ b/Lojas/Juntando Tudo/Enderecos_Processados.xlsx
@@ -455,11 +455,6 @@
           <t>Barris</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -507,11 +502,6 @@
           <t>Federação</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -559,11 +549,6 @@
           <t>Vila Laura</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -611,11 +596,6 @@
           <t>Luís Anselmo</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -663,11 +643,6 @@
           <t>Uruguai</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -715,11 +690,6 @@
           <t>Bonocô</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -762,11 +732,6 @@
           <t>Granjas Rurais Pres. Vargas</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -814,11 +779,6 @@
           <t>Cabula</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -866,11 +826,6 @@
           <t>Loja Trecho A</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -918,11 +873,6 @@
           <t>Cabula</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -970,11 +920,6 @@
           <t>Pau da Lima</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1022,11 +967,6 @@
           <t>Liberdade</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1069,16 +1009,6 @@
           <t>R. Nilo Peçanha, 9/11</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>- 9/11 - Calçada</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1121,11 +1051,6 @@
           <t>Granjas Rurais Pres. Vargas</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1220,11 +1145,6 @@
           <t>Boca do Rio</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1272,11 +1192,6 @@
           <t>Av. Sete de Setembro</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1356,11 +1271,6 @@
           <t>Daniel Lisboa</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1403,11 +1313,6 @@
           <t>Garcia</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1450,11 +1355,6 @@
           <t>Engenho Velho da Federação</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1492,11 +1392,6 @@
           <t>Engenho Velho da Federacao</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1534,11 +1429,6 @@
           <t>Tororo</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1581,11 +1471,6 @@
           <t>Liberdade</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1633,11 +1518,6 @@
           <t>Graça</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1685,11 +1565,6 @@
           <t>Federação</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1727,11 +1602,6 @@
           <t>Federação</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1868,11 +1738,6 @@
           <t>Av. Joana Angélica</t>
         </is>
       </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1957,11 +1822,6 @@
           <t>Centro</t>
         </is>
       </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2004,11 +1864,6 @@
           <t>´RUA SERGIO DE CARVALHO</t>
         </is>
       </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2098,11 +1953,6 @@
           <t>Barra</t>
         </is>
       </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2150,11 +2000,6 @@
           <t>Rio Vermelho</t>
         </is>
       </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2192,11 +2037,6 @@
           <t>Tororo</t>
         </is>
       </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2234,11 +2074,6 @@
           <t>Iapi</t>
         </is>
       </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2390,11 +2225,6 @@
           <t>Barris</t>
         </is>
       </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2437,11 +2267,6 @@
           <t>Av. Sete de Setembro</t>
         </is>
       </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2516,11 +2341,6 @@
           <t>Barris</t>
         </is>
       </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2563,11 +2383,6 @@
           <t>Av. Dom João VI</t>
         </is>
       </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2615,11 +2430,6 @@
           <t>Brotas</t>
         </is>
       </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2662,11 +2472,6 @@
           <t>Barris</t>
         </is>
       </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2694,16 +2499,6 @@
           <t>R. Djalma Dutra, 637</t>
         </is>
       </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>- 1o Andar - Matatu</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2746,11 +2541,6 @@
           <t>Garcia</t>
         </is>
       </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2788,11 +2578,6 @@
           <t>Campo Grande</t>
         </is>
       </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2830,11 +2615,6 @@
           <t>Tororo</t>
         </is>
       </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2882,11 +2662,6 @@
           <t>Garcia</t>
         </is>
       </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2976,11 +2751,6 @@
           <t>Nazaré</t>
         </is>
       </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3018,11 +2788,6 @@
           <t>Centro</t>
         </is>
       </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3065,11 +2830,6 @@
           <t>Av. Sete de Setembro</t>
         </is>
       </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3107,11 +2867,6 @@
           <t>Campo Grande</t>
         </is>
       </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3154,11 +2909,6 @@
           <t>Fazenda Garcia</t>
         </is>
       </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3201,11 +2951,6 @@
           <t>Engenho Velho de Brotas</t>
         </is>
       </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3290,11 +3035,6 @@
           <t>Daniel Lisboa</t>
         </is>
       </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3337,11 +3077,6 @@
           <t>Brotas</t>
         </is>
       </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3384,11 +3119,6 @@
           <t>Pituba</t>
         </is>
       </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3431,11 +3161,6 @@
           <t>Engenho Velho de Brotas</t>
         </is>
       </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3557,11 +3282,6 @@
           <t>Acupe de Brotas</t>
         </is>
       </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3604,11 +3324,6 @@
           <t>Engenho Velho de Brotas</t>
         </is>
       </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3646,11 +3361,6 @@
           <t>Dois de Julho</t>
         </is>
       </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3799,11 +3509,6 @@
           <t>Centro</t>
         </is>
       </c>
-      <c r="J74" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3841,11 +3546,6 @@
           <t>Baixa dos Sapateiros</t>
         </is>
       </c>
-      <c r="J75" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4046,11 +3746,6 @@
           <t>Brotas</t>
         </is>
       </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -4098,11 +3793,6 @@
           <t>Engenho Velho de Brotas</t>
         </is>
       </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -4145,11 +3835,6 @@
           <t>Brotas</t>
         </is>
       </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -4192,11 +3877,6 @@
           <t>Largo do Campo da Pólvora</t>
         </is>
       </c>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -4234,11 +3914,6 @@
           <t>Boa Vista De Brotas</t>
         </is>
       </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -4281,11 +3956,6 @@
           <t>Área Limite da BCS Calabar</t>
         </is>
       </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -4407,11 +4077,6 @@
           <t>Brotas</t>
         </is>
       </c>
-      <c r="J88" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -4476,16 +4141,6 @@
           <t>Av. Mário Leal Ferreira, 780</t>
         </is>
       </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>- Loja B 520 - Daniel Lisboa</t>
-        </is>
-      </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -4528,11 +4183,6 @@
           <t>Garcia</t>
         </is>
       </c>
-      <c r="J91" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -4617,11 +4267,6 @@
           <t>Tororo</t>
         </is>
       </c>
-      <c r="J93" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4659,16 +4304,6 @@
           <t>R. Eng. Silva Lima, no 117</t>
         </is>
       </c>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>- Térreo - Nazaré</t>
-        </is>
-      </c>
-      <c r="J94" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4775,11 +4410,6 @@
           <t>Cardeal da Silva</t>
         </is>
       </c>
-      <c r="J97" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4827,11 +4457,6 @@
           <t>Daniel Lisboa</t>
         </is>
       </c>
-      <c r="J98" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4891,16 +4516,6 @@
           <t>Av. Tancredo Neves, 939</t>
         </is>
       </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>- Sala 904 - Caminho das Árvores</t>
-        </is>
-      </c>
-      <c r="J100" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4943,11 +4558,6 @@
           <t>Rio Vermelho</t>
         </is>
       </c>
-      <c r="J101" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4985,11 +4595,6 @@
           <t>Brotas</t>
         </is>
       </c>
-      <c r="J102" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -5059,11 +4664,6 @@
           <t>Calçada</t>
         </is>
       </c>
-      <c r="J104" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -5106,11 +4706,6 @@
           <t>Comercio</t>
         </is>
       </c>
-      <c r="J105" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -5153,16 +4748,6 @@
           <t>Shopping Piedade</t>
         </is>
       </c>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>- Barris</t>
-        </is>
-      </c>
-      <c r="J106" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -5205,11 +4790,6 @@
           <t>Av. Dom João VI</t>
         </is>
       </c>
-      <c r="J107" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -5252,16 +4832,6 @@
           <t>Av. Gen. Graça Lessa, 1179</t>
         </is>
       </c>
-      <c r="I108" t="inlineStr">
-        <is>
-          <t>- F - Engenho Velho de Brotas</t>
-        </is>
-      </c>
-      <c r="J108" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -5321,16 +4891,6 @@
           <t>BR</t>
         </is>
       </c>
-      <c r="I110" t="inlineStr">
-        <is>
-          <t>- KM 7 - Pirajá</t>
-        </is>
-      </c>
-      <c r="J110" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -5373,16 +4933,6 @@
           <t>Avenida Tancredo Neves</t>
         </is>
       </c>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>Loja 5015 - Caminho das Árvores</t>
-        </is>
-      </c>
-      <c r="J111" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -5462,11 +5012,6 @@
           <t>Comercio</t>
         </is>
       </c>
-      <c r="J113" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -5635,11 +5180,6 @@
           <t>Saboeiro</t>
         </is>
       </c>
-      <c r="J117" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -5682,16 +5222,6 @@
           <t>Av. Tancredo Neves, 3133</t>
         </is>
       </c>
-      <c r="I118" t="inlineStr">
-        <is>
-          <t>- 1º Andar - Caminho das Árvores</t>
-        </is>
-      </c>
-      <c r="J118" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -5734,11 +5264,6 @@
           <t>Periperi</t>
         </is>
       </c>
-      <c r="J119" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -5818,11 +5343,6 @@
           <t>Iapi</t>
         </is>
       </c>
-      <c r="J121" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -5865,11 +5385,6 @@
           <t>Comercio</t>
         </is>
       </c>
-      <c r="J122" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -5912,11 +5427,6 @@
           <t>Pituba</t>
         </is>
       </c>
-      <c r="J123" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -6048,11 +5558,6 @@
           <t>Horto Florestal</t>
         </is>
       </c>
-      <c r="J126" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -6142,11 +5647,6 @@
           <t>Mares</t>
         </is>
       </c>
-      <c r="J128" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -6189,11 +5689,6 @@
           <t>Av. Sete de Setembro</t>
         </is>
       </c>
-      <c r="J129" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -6241,11 +5736,6 @@
           <t>Recreio Ipitanga</t>
         </is>
       </c>
-      <c r="J130" t="inlineStr">
-        <is>
-          <t>Lauro de Freitas</t>
-        </is>
-      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -6293,11 +5783,6 @@
           <t>São Marcos</t>
         </is>
       </c>
-      <c r="J131" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -6345,11 +5830,6 @@
           <t>Dois de Julho</t>
         </is>
       </c>
-      <c r="J132" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -6397,11 +5877,6 @@
           <t>Itapuã</t>
         </is>
       </c>
-      <c r="J133" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -6491,11 +5966,6 @@
           <t>Horto Bela Vista</t>
         </is>
       </c>
-      <c r="J135" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -6538,11 +6008,6 @@
           <t>Barris</t>
         </is>
       </c>
-      <c r="J136" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -6590,11 +6055,6 @@
           <t>Piedade</t>
         </is>
       </c>
-      <c r="J137" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -6632,16 +6092,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I138" t="inlineStr">
-        <is>
-          <t>- Loja 277 - Barra</t>
-        </is>
-      </c>
-      <c r="J138" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -6679,16 +6129,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I139" t="inlineStr">
-        <is>
-          <t>- Loja 62 - Barra</t>
-        </is>
-      </c>
-      <c r="J139" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -6731,11 +6171,6 @@
           <t>Piedade</t>
         </is>
       </c>
-      <c r="J140" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -6778,16 +6213,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I141" t="inlineStr">
-        <is>
-          <t>- Loja 155 - Barra</t>
-        </is>
-      </c>
-      <c r="J141" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -6825,16 +6250,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I142" t="inlineStr">
-        <is>
-          <t>- Loja 5 - Barra</t>
-        </is>
-      </c>
-      <c r="J142" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -6877,11 +6292,6 @@
           <t>Itaigara</t>
         </is>
       </c>
-      <c r="J143" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -6929,11 +6339,6 @@
           <t>Barris</t>
         </is>
       </c>
-      <c r="J144" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -6981,11 +6386,6 @@
           <t>Caminho das Árvores</t>
         </is>
       </c>
-      <c r="J145" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -7023,16 +6423,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I146" t="inlineStr">
-        <is>
-          <t>- Loja 87 - Barra</t>
-        </is>
-      </c>
-      <c r="J146" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -7075,16 +6465,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I147" t="inlineStr">
-        <is>
-          <t>- Loja 278 - Barra</t>
-        </is>
-      </c>
-      <c r="J147" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -7122,16 +6502,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I148" t="inlineStr">
-        <is>
-          <t>- Chame-Chame</t>
-        </is>
-      </c>
-      <c r="J148" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -7174,11 +6544,6 @@
           <t>Caminho das Árvores</t>
         </is>
       </c>
-      <c r="J149" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -7221,11 +6586,6 @@
           <t>Caminho das Árvores</t>
         </is>
       </c>
-      <c r="J150" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -7268,16 +6628,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I151" t="inlineStr">
-        <is>
-          <t>- Loja 273 - Barra</t>
-        </is>
-      </c>
-      <c r="J151" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -7315,16 +6665,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I152" t="inlineStr">
-        <is>
-          <t>- Loja 141 - Barra</t>
-        </is>
-      </c>
-      <c r="J152" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -7367,16 +6707,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I153" t="inlineStr">
-        <is>
-          <t>- Loja 2 - Barra</t>
-        </is>
-      </c>
-      <c r="J153" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -7424,11 +6754,6 @@
           <t>Caminho das Árvores</t>
         </is>
       </c>
-      <c r="J154" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -7476,11 +6801,6 @@
           <t>Caminho das Árvores</t>
         </is>
       </c>
-      <c r="J155" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -7518,16 +6838,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I156" t="inlineStr">
-        <is>
-          <t>- Loja 75 - Barra</t>
-        </is>
-      </c>
-      <c r="J156" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -7570,16 +6880,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I157" t="inlineStr">
-        <is>
-          <t>- Chame-Chame</t>
-        </is>
-      </c>
-      <c r="J157" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -7617,16 +6917,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I158" t="inlineStr">
-        <is>
-          <t>- Loja 272 - Barra</t>
-        </is>
-      </c>
-      <c r="J158" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -7669,16 +6959,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I159" t="inlineStr">
-        <is>
-          <t>- Loja 235 - Barra</t>
-        </is>
-      </c>
-      <c r="J159" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -7716,16 +6996,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I160" t="inlineStr">
-        <is>
-          <t>- Loja 15 - Barra</t>
-        </is>
-      </c>
-      <c r="J160" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -7763,16 +7033,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I161" t="inlineStr">
-        <is>
-          <t>- Loja 152 - Barra</t>
-        </is>
-      </c>
-      <c r="J161" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -7815,16 +7075,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I162" t="inlineStr">
-        <is>
-          <t>- Loja 82 - Barra</t>
-        </is>
-      </c>
-      <c r="J162" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -7862,16 +7112,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I163" t="inlineStr">
-        <is>
-          <t>- Loja 56 - Barra</t>
-        </is>
-      </c>
-      <c r="J163" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -7919,11 +7159,6 @@
           <t>Itaigara</t>
         </is>
       </c>
-      <c r="J164" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -7966,11 +7201,6 @@
           <t>São Caetano</t>
         </is>
       </c>
-      <c r="J165" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -8013,11 +7243,6 @@
           <t>Jardim Apipema</t>
         </is>
       </c>
-      <c r="J166" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -8055,16 +7280,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I167" t="inlineStr">
-        <is>
-          <t>- Loja 124 - Barra</t>
-        </is>
-      </c>
-      <c r="J167" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -8107,16 +7322,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I168" t="inlineStr">
-        <is>
-          <t>- Loja 154 - Barra</t>
-        </is>
-      </c>
-      <c r="J168" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -8154,16 +7359,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I169" t="inlineStr">
-        <is>
-          <t>- Loja 135 - Barra</t>
-        </is>
-      </c>
-      <c r="J169" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -8206,16 +7401,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I170" t="inlineStr">
-        <is>
-          <t>- Loja 217 - Barra</t>
-        </is>
-      </c>
-      <c r="J170" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -8263,11 +7448,6 @@
           <t>Alameda Euvaldo Luz</t>
         </is>
       </c>
-      <c r="J171" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -8310,16 +7490,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I172" t="inlineStr">
-        <is>
-          <t>- Loja 7 - Barra</t>
-        </is>
-      </c>
-      <c r="J172" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -8362,16 +7532,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I173" t="inlineStr">
-        <is>
-          <t>- Loja 261 - Barra</t>
-        </is>
-      </c>
-      <c r="J173" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -8409,16 +7569,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I174" t="inlineStr">
-        <is>
-          <t>- Loja 119 - Barra</t>
-        </is>
-      </c>
-      <c r="J174" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -8461,16 +7611,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I175" t="inlineStr">
-        <is>
-          <t>- loja 352/353 - Barra</t>
-        </is>
-      </c>
-      <c r="J175" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -8518,11 +7658,6 @@
           <t>Horto Bela Vista</t>
         </is>
       </c>
-      <c r="J176" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -8565,16 +7700,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I177" t="inlineStr">
-        <is>
-          <t>- Loja 71 - Barra</t>
-        </is>
-      </c>
-      <c r="J177" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -8612,16 +7737,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I178" t="inlineStr">
-        <is>
-          <t>- Loja 10 - Barra</t>
-        </is>
-      </c>
-      <c r="J178" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -8669,11 +7784,6 @@
           <t>Av. Centenário</t>
         </is>
       </c>
-      <c r="J179" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -8711,16 +7821,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I180" t="inlineStr">
-        <is>
-          <t>- Loja 63 - Barra</t>
-        </is>
-      </c>
-      <c r="J180" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -8758,16 +7858,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I181" t="inlineStr">
-        <is>
-          <t>- Loja 437 - Barra</t>
-        </is>
-      </c>
-      <c r="J181" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -8805,16 +7895,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I182" t="inlineStr">
-        <is>
-          <t>- Loja 274 - Barra</t>
-        </is>
-      </c>
-      <c r="J182" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -8847,11 +7927,6 @@
           <t>Centro</t>
         </is>
       </c>
-      <c r="J183" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -8894,16 +7969,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I184" t="inlineStr">
-        <is>
-          <t>- Loja 275 - Barra</t>
-        </is>
-      </c>
-      <c r="J184" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -8951,11 +8016,6 @@
           <t>Caminho das Árvores</t>
         </is>
       </c>
-      <c r="J185" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -8993,16 +8053,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I186" t="inlineStr">
-        <is>
-          <t>- Loja 184 - Barra</t>
-        </is>
-      </c>
-      <c r="J186" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -9045,11 +8095,6 @@
           <t>Comercio</t>
         </is>
       </c>
-      <c r="J187" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -9097,11 +8142,6 @@
           <t>Dois de Julho</t>
         </is>
       </c>
-      <c r="J188" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -9149,11 +8189,6 @@
           <t>Dois de Julho</t>
         </is>
       </c>
-      <c r="J189" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -9201,11 +8236,6 @@
           <t>Av. Centenário</t>
         </is>
       </c>
-      <c r="J190" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -9243,16 +8273,6 @@
           <t>Av. Tancredo Neves, 3133</t>
         </is>
       </c>
-      <c r="I191" t="inlineStr">
-        <is>
-          <t>- 208 - Caminho das Árvores</t>
-        </is>
-      </c>
-      <c r="J191" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -9290,16 +8310,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I192" t="inlineStr">
-        <is>
-          <t>- Loja 280 - Barra</t>
-        </is>
-      </c>
-      <c r="J192" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -9337,16 +8347,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I193" t="inlineStr">
-        <is>
-          <t>- Loja 245 - Barra</t>
-        </is>
-      </c>
-      <c r="J193" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -9394,11 +8394,6 @@
           <t>Castelo Branco</t>
         </is>
       </c>
-      <c r="J194" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -9436,16 +8431,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I195" t="inlineStr">
-        <is>
-          <t>- Loja 53 - Barra</t>
-        </is>
-      </c>
-      <c r="J195" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -9493,11 +8478,6 @@
           <t>Shopping</t>
         </is>
       </c>
-      <c r="J196" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -9535,16 +8515,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I197" t="inlineStr">
-        <is>
-          <t>- Loja 38 - Barra</t>
-        </is>
-      </c>
-      <c r="J197" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -9587,11 +8557,6 @@
           <t>Pau da Lima</t>
         </is>
       </c>
-      <c r="J198" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -9629,16 +8594,6 @@
           <t>R. Conde de Porto Alegre, 93</t>
         </is>
       </c>
-      <c r="I199" t="inlineStr">
-        <is>
-          <t>- OT - Iapi</t>
-        </is>
-      </c>
-      <c r="J199" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -9681,11 +8636,6 @@
           <t>Liberdade</t>
         </is>
       </c>
-      <c r="J200" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -9723,16 +8673,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I201" t="inlineStr">
-        <is>
-          <t>- Loja 164 - Barra</t>
-        </is>
-      </c>
-      <c r="J201" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -9775,11 +8715,6 @@
           <t>Pituba</t>
         </is>
       </c>
-      <c r="J202" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -9864,16 +8799,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I204" t="inlineStr">
-        <is>
-          <t>- Loja 209 - Barra</t>
-        </is>
-      </c>
-      <c r="J204" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -9916,16 +8841,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I205" t="inlineStr">
-        <is>
-          <t>- Loja 293 - Barra</t>
-        </is>
-      </c>
-      <c r="J205" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -9973,11 +8888,6 @@
           <t>Comercio</t>
         </is>
       </c>
-      <c r="J206" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -10010,16 +8920,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I207" t="inlineStr">
-        <is>
-          <t>- Loja 192 - Barra</t>
-        </is>
-      </c>
-      <c r="J207" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -10104,11 +9004,6 @@
           <t>Calçada</t>
         </is>
       </c>
-      <c r="J209" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -10151,16 +9046,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I210" t="inlineStr">
-        <is>
-          <t>- Loja 190 - Barra</t>
-        </is>
-      </c>
-      <c r="J210" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -10208,11 +9093,6 @@
           <t>Estr. da Liberdade</t>
         </is>
       </c>
-      <c r="J211" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -10255,16 +9135,6 @@
           <t>Rua Barão de Cotegipe, 92</t>
         </is>
       </c>
-      <c r="I212" t="inlineStr">
-        <is>
-          <t>- E 94 - Calçada</t>
-        </is>
-      </c>
-      <c r="J212" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -10307,16 +9177,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I213" t="inlineStr">
-        <is>
-          <t>- Loja 92 - Barra</t>
-        </is>
-      </c>
-      <c r="J213" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -10364,11 +9224,6 @@
           <t>Comercio</t>
         </is>
       </c>
-      <c r="J214" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -10401,16 +9256,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I215" t="inlineStr">
-        <is>
-          <t>- Loja 215 - Barra</t>
-        </is>
-      </c>
-      <c r="J215" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -10448,16 +9293,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I216" t="inlineStr">
-        <is>
-          <t>- Loja 49 - Barra</t>
-        </is>
-      </c>
-      <c r="J216" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -10495,16 +9330,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I217" t="inlineStr">
-        <is>
-          <t>- Loja 26 - Barra</t>
-        </is>
-      </c>
-      <c r="J217" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -10542,16 +9367,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I218" t="inlineStr">
-        <is>
-          <t>- Loja 76 - Barra</t>
-        </is>
-      </c>
-      <c r="J218" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -10594,16 +9409,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I219" t="inlineStr">
-        <is>
-          <t>- Loja 171 - Barra</t>
-        </is>
-      </c>
-      <c r="J219" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -10651,11 +9456,6 @@
           <t>Calçada</t>
         </is>
       </c>
-      <c r="J220" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -10698,11 +9498,6 @@
           <t>Comercio</t>
         </is>
       </c>
-      <c r="J221" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -10777,16 +9572,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I223" t="inlineStr">
-        <is>
-          <t>- Loja 260 - Barra</t>
-        </is>
-      </c>
-      <c r="J223" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -10834,11 +9619,6 @@
           <t>São Cristóvão</t>
         </is>
       </c>
-      <c r="J224" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -10876,16 +9656,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I225" t="inlineStr">
-        <is>
-          <t>- Loja 105 - Barra</t>
-        </is>
-      </c>
-      <c r="J225" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -10928,16 +9698,6 @@
           <t>Estr. da Paciência, 1400</t>
         </is>
       </c>
-      <c r="I226" t="inlineStr">
-        <is>
-          <t>- Cajazeiras 8</t>
-        </is>
-      </c>
-      <c r="J226" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -10975,16 +9735,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I227" t="inlineStr">
-        <is>
-          <t>- Loja 221 - Barra</t>
-        </is>
-      </c>
-      <c r="J227" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -11022,16 +9772,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I228" t="inlineStr">
-        <is>
-          <t>- Loja 228 - Barra</t>
-        </is>
-      </c>
-      <c r="J228" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -11069,16 +9809,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I229" t="inlineStr">
-        <is>
-          <t>- Loja 287 - Barra</t>
-        </is>
-      </c>
-      <c r="J229" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -11126,11 +9856,6 @@
           <t>Itaigara</t>
         </is>
       </c>
-      <c r="J230" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -11173,16 +9898,6 @@
           <t>Av. Centenário, 2992</t>
         </is>
       </c>
-      <c r="I231" t="inlineStr">
-        <is>
-          <t>- Loja 181 - Barra</t>
-        </is>
-      </c>
-      <c r="J231" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -11230,11 +9945,6 @@
           <t>Engenho Velho de Brotas</t>
         </is>
       </c>
-      <c r="J232" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -11272,16 +9982,6 @@
           <t>Rua Conselheiro Junqueira Ayres, 165</t>
         </is>
       </c>
-      <c r="I233" t="inlineStr">
-        <is>
-          <t>- 58 - Barris</t>
-        </is>
-      </c>
-      <c r="J233" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -11371,11 +10071,6 @@
           <t>Centro</t>
         </is>
       </c>
-      <c r="J235" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -11423,11 +10118,6 @@
           <t>Dois de Julho</t>
         </is>
       </c>
-      <c r="J236" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -11465,11 +10155,6 @@
           <t>Campo Grande</t>
         </is>
       </c>
-      <c r="J237" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -11507,11 +10192,6 @@
           <t>Luís Anselmo</t>
         </is>
       </c>
-      <c r="J238" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -11554,11 +10234,6 @@
           <t>R. Nossa Sra. do Resgate</t>
         </is>
       </c>
-      <c r="J239" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -11596,16 +10271,6 @@
           <t>R. Portão da Piedade, 155</t>
         </is>
       </c>
-      <c r="I240" t="inlineStr">
-        <is>
-          <t>- 223 - Barris</t>
-        </is>
-      </c>
-      <c r="J240" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -11653,11 +10318,6 @@
           <t>Av. Dom João VI</t>
         </is>
       </c>
-      <c r="J241" t="inlineStr">
-        <is>
-          <t>342</t>
-        </is>
-      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -11700,11 +10360,6 @@
           <t>Nazaré</t>
         </is>
       </c>
-      <c r="J242" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -11752,11 +10407,6 @@
           <t>Barris</t>
         </is>
       </c>
-      <c r="J243" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -11799,11 +10449,6 @@
           <t>R. da Paz</t>
         </is>
       </c>
-      <c r="J244" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -11841,16 +10486,6 @@
           <t>Av. Dom João VI, 1050</t>
         </is>
       </c>
-      <c r="I245" t="inlineStr">
-        <is>
-          <t>- Shopping Brotascenter - Brotas</t>
-        </is>
-      </c>
-      <c r="J245" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -11898,11 +10533,6 @@
           <t>Dois de Julho</t>
         </is>
       </c>
-      <c r="J246" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -11940,16 +10570,6 @@
           <t>Av. Tancredo Neves, 3133</t>
         </is>
       </c>
-      <c r="I247" t="inlineStr">
-        <is>
-          <t>- 106 - Caminho das Árvores</t>
-        </is>
-      </c>
-      <c r="J247" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -11992,11 +10612,6 @@
           <t>Boca do Rio</t>
         </is>
       </c>
-      <c r="J248" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -12044,11 +10659,6 @@
           <t>Nazaré</t>
         </is>
       </c>
-      <c r="J249" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -12091,11 +10701,6 @@
           <t>Av. Sete de Setembro</t>
         </is>
       </c>
-      <c r="J250" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -12138,11 +10743,6 @@
           <t>Nazaré</t>
         </is>
       </c>
-      <c r="J251" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -12180,11 +10780,6 @@
           <t>Federação</t>
         </is>
       </c>
-      <c r="J252" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -12232,11 +10827,6 @@
           <t>Armação</t>
         </is>
       </c>
-      <c r="J253" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -12279,11 +10869,6 @@
           <t>Ondina</t>
         </is>
       </c>
-      <c r="J254" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -12321,11 +10906,6 @@
           <t>Av. José Joaquim Seabra</t>
         </is>
       </c>
-      <c r="J255" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -12420,11 +11000,6 @@
           <t>Barroquinha</t>
         </is>
       </c>
-      <c r="J257" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -12472,11 +11047,6 @@
           <t>Brotas</t>
         </is>
       </c>
-      <c r="J258" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -12514,11 +11084,6 @@
           <t>Av. Sete de Setembro</t>
         </is>
       </c>
-      <c r="J259" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -12561,11 +11126,6 @@
           <t>Barris</t>
         </is>
       </c>
-      <c r="J260" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -12645,16 +11205,6 @@
           <t>R. João Gomes, 87</t>
         </is>
       </c>
-      <c r="I262" t="inlineStr">
-        <is>
-          <t>- Loja 3B - Rio Vermelho</t>
-        </is>
-      </c>
-      <c r="J262" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -12697,11 +11247,6 @@
           <t>Imbuí</t>
         </is>
       </c>
-      <c r="J263" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -12796,11 +11341,6 @@
           <t>Engenho Velho de Brotas</t>
         </is>
       </c>
-      <c r="J265" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -12838,11 +11378,6 @@
           <t>Garcia</t>
         </is>
       </c>
-      <c r="J266" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -12890,11 +11425,6 @@
           <t>Tororo</t>
         </is>
       </c>
-      <c r="J267" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -12932,11 +11462,6 @@
           <t>Engenho Velho de Brotas</t>
         </is>
       </c>
-      <c r="J268" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -12979,16 +11504,6 @@
           <t>Av. Dom João VI, 177</t>
         </is>
       </c>
-      <c r="I269" t="inlineStr">
-        <is>
-          <t>- galeria - Santa Teresa</t>
-        </is>
-      </c>
-      <c r="J269" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -13068,16 +11583,6 @@
           <t>R. Barão de Loreto, 08</t>
         </is>
       </c>
-      <c r="I271" t="inlineStr">
-        <is>
-          <t>- loja 03 - Graça</t>
-        </is>
-      </c>
-      <c r="J271" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -13120,11 +11625,6 @@
           <t>Barris</t>
         </is>
       </c>
-      <c r="J272" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -13167,11 +11667,6 @@
           <t>Nazaré</t>
         </is>
       </c>
-      <c r="J273" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -13219,11 +11714,6 @@
           <t>Piedade</t>
         </is>
       </c>
-      <c r="J274" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -13313,11 +11803,6 @@
           <t>Nazaré</t>
         </is>
       </c>
-      <c r="J276" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -13355,11 +11840,6 @@
           <t>Tororo</t>
         </is>
       </c>
-      <c r="J277" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -13402,11 +11882,6 @@
           <t>Engenho Velho de Brotas</t>
         </is>
       </c>
-      <c r="J278" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -13454,11 +11929,6 @@
           <t>Garcia</t>
         </is>
       </c>
-      <c r="J279" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -13501,11 +11971,6 @@
           <t>Engenho Velho de Brotas</t>
         </is>
       </c>
-      <c r="J280" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -13543,16 +12008,6 @@
           <t>R. Gen. Labatut, 137</t>
         </is>
       </c>
-      <c r="I281" t="inlineStr">
-        <is>
-          <t>- 17 - Barris</t>
-        </is>
-      </c>
-      <c r="J281" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -13647,11 +12102,6 @@
           <t>Nazaré</t>
         </is>
       </c>
-      <c r="J283" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -13699,11 +12149,6 @@
           <t>Dois de Julho</t>
         </is>
       </c>
-      <c r="J284" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -13840,11 +12285,6 @@
           <t>Acupe</t>
         </is>
       </c>
-      <c r="J287" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -13887,11 +12327,6 @@
           <t>Engenho Velho da Federacao</t>
         </is>
       </c>
-      <c r="J288" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -13986,11 +12421,6 @@
           <t>Sobre loja</t>
         </is>
       </c>
-      <c r="J290" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -14033,11 +12463,6 @@
           <t>Nazaré</t>
         </is>
       </c>
-      <c r="J291" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -14085,11 +12510,6 @@
           <t>Dois de Julho</t>
         </is>
       </c>
-      <c r="J292" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -14132,11 +12552,6 @@
           <t>Rua Conselheiro Junqueira Ayres</t>
         </is>
       </c>
-      <c r="J293" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -14184,11 +12599,6 @@
           <t>Centro</t>
         </is>
       </c>
-      <c r="J294" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -14236,11 +12646,6 @@
           <t>Brotas</t>
         </is>
       </c>
-      <c r="J295" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -14288,11 +12693,6 @@
           <t>Engenho Velho de Brotas</t>
         </is>
       </c>
-      <c r="J296" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -14330,11 +12730,6 @@
           <t>Engenho Velho da Federação</t>
         </is>
       </c>
-      <c r="J297" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -14419,11 +12814,6 @@
           <t>Garcia</t>
         </is>
       </c>
-      <c r="J299" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -14461,11 +12851,6 @@
           <t>Piedade</t>
         </is>
       </c>
-      <c r="J300" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -14513,11 +12898,6 @@
           <t>Piedade</t>
         </is>
       </c>
-      <c r="J301" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -14565,11 +12945,6 @@
           <t>Dois de Julho</t>
         </is>
       </c>
-      <c r="J302" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -14617,11 +12992,6 @@
           <t>Engenho Velho da Federacao</t>
         </is>
       </c>
-      <c r="J303" t="inlineStr">
-        <is>
-          <t>Salvador</t>
-        </is>
-      </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -14709,11 +13079,6 @@
       <c r="I305" t="inlineStr">
         <is>
           <t>Horto Florestal</t>
-        </is>
-      </c>
-      <c r="J305" t="inlineStr">
-        <is>
-          <t>Salvador</t>
         </is>
       </c>
     </row>

</xml_diff>